<commit_message>
Work on worksheet two
</commit_message>
<xml_diff>
--- a/WorksheetTwo/NewExcelFile.xlsx
+++ b/WorksheetTwo/NewExcelFile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="o:\Classes\IS\Practical\WorksheetTwo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Classes\IS\Practical\WorksheetTwo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB5C69A-93A1-4674-B2F4-986326E3A2A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F87BAAF-E2D3-4D05-8710-D18CC46228CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" activeTab="4" xr2:uid="{DDFB8BC9-3EF7-4211-9502-C349FF4A5F91}"/>
+    <workbookView xWindow="9150" yWindow="2655" windowWidth="28800" windowHeight="15435" xr2:uid="{DDFB8BC9-3EF7-4211-9502-C349FF4A5F91}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Worksheet</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>Five!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdasdasdsda_x000D_
+asd_x000D_
+asd_x000D_
+</t>
   </si>
 </sst>
 </file>
@@ -91,8 +97,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -108,6 +117,435 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Graph Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Folha1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C66B-4856-8BD0-C09134F4DCEF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1764716768"/>
+        <c:axId val="1764706368"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1764716768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Title of X axis</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1764706368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1764706368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Title of Y axis</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1764716768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Graph Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Folha1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8BC2-42AA-8CC5-B1F235FF0F68}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2017649055"/>
+        <c:axId val="2017653631"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2017649055"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Title of X axis</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2017653631"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2017653631"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Title of Y axis</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2017649055"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>187325</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>339725</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1DE32C0-CF56-4E38-9114-8D193D1A667E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>34925</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>187325</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13FEB79B-A28C-461D-B61B-6E21DF7F1E4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,22 +845,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B41148-84B5-4847-B029-C3CB5F867AC9}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -497,7 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF47CD27-4987-46DE-848C-04974048A69A}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Make some UI changes
</commit_message>
<xml_diff>
--- a/WorksheetTwo/NewExcelFile.xlsx
+++ b/WorksheetTwo/NewExcelFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Classes\IS\Practical\WorksheetTwo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F87BAAF-E2D3-4D05-8710-D18CC46228CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7254E0-A59F-4CFB-8344-DAAAE235586D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9150" yWindow="2655" windowWidth="28800" windowHeight="15435" xr2:uid="{DDFB8BC9-3EF7-4211-9502-C349FF4A5F91}"/>
+    <workbookView xWindow="5310" yWindow="3090" windowWidth="28800" windowHeight="15435" xr2:uid="{DDFB8BC9-3EF7-4211-9502-C349FF4A5F91}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Worksheet</t>
   </si>
@@ -56,12 +56,6 @@
   </si>
   <si>
     <t>Five!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asdasdasdsda_x000D_
-asd_x000D_
-asd_x000D_
-</t>
   </si>
 </sst>
 </file>
@@ -471,6 +465,182 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Graph Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Folha1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>one!</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Folha1!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2B77-423F-8551-194AC4451A2B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1209250416"/>
+        <c:axId val="1209252912"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1209250416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Title of X axis</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1209252912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1209252912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Title of Y axis</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1209250416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -540,6 +710,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>187325</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>339725</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BC39AD4-35C9-4AB0-8BC8-EE3E4D4FD823}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -848,14 +1054,14 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -883,12 +1089,12 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>